<commit_message>
new file: barcode generator for labels
</commit_message>
<xml_diff>
--- a/Server/Teszt/MesterLista.xlsx
+++ b/Server/Teszt/MesterLista.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Megosztott mappa\Kutatók Éjszakája\Teszt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progik\3DPuzzleQuiz\Server\Teszt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1840,22 +1840,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="24" style="10" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="24" style="10" customWidth="1"/>
-    <col min="7" max="8" width="11.28515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="3" customWidth="1"/>
-    <col min="10" max="16" width="8.7109375" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="38.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="10" customWidth="1"/>
+    <col min="7" max="8" width="11.140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="3" customWidth="1"/>
+    <col min="10" max="11" width="8.7109375" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,19 +1863,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>6</v>
@@ -1892,19 +1892,19 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>15</v>
@@ -1921,19 +1921,19 @@
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>21</v>
@@ -1950,19 +1950,19 @@
         <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>29</v>
@@ -1979,19 +1979,19 @@
         <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>35</v>
@@ -2008,19 +2008,19 @@
         <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>41</v>
@@ -2037,19 +2037,19 @@
         <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>45</v>
@@ -2066,19 +2066,19 @@
         <v>47</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>53</v>
@@ -2095,19 +2095,19 @@
         <v>55</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>61</v>
@@ -2124,19 +2124,19 @@
         <v>63</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>65</v>
@@ -2153,19 +2153,19 @@
         <v>67</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>69</v>
@@ -2180,19 +2180,19 @@
         <v>70</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>72</v>
@@ -2209,19 +2209,19 @@
         <v>74</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>77</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>79</v>
@@ -2238,19 +2238,19 @@
         <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>84</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>86</v>
@@ -2267,19 +2267,19 @@
         <v>88</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>93</v>
@@ -2296,19 +2296,19 @@
         <v>95</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>97</v>
@@ -2325,19 +2325,19 @@
         <v>98</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>98</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>102</v>
@@ -2352,19 +2352,19 @@
         <v>103</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>103</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>104</v>
@@ -2379,19 +2379,19 @@
         <v>105</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>105</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>107</v>
@@ -2408,19 +2408,19 @@
         <v>109</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>109</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>110</v>
@@ -2437,19 +2437,19 @@
         <v>112</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>112</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>117</v>
@@ -2466,19 +2466,19 @@
         <v>119</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>122</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>125</v>
@@ -2495,19 +2495,19 @@
         <v>127</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>130</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>132</v>
@@ -2524,19 +2524,19 @@
         <v>134</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>136</v>
@@ -2551,19 +2551,19 @@
         <v>137</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>137</v>
       </c>
       <c r="E25" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>138</v>
@@ -2580,19 +2580,19 @@
         <v>139</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E26" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>141</v>
@@ -2609,19 +2609,19 @@
         <v>143</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>145</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>146</v>
@@ -2638,19 +2638,19 @@
         <v>148</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>149</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>150</v>
@@ -2665,19 +2665,19 @@
         <v>151</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>152</v>
       </c>
       <c r="E29" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>153</v>
@@ -2692,19 +2692,19 @@
         <v>154</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>156</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>157</v>
@@ -2721,19 +2721,19 @@
         <v>159</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>160</v>
       </c>
       <c r="E31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>161</v>
@@ -2750,19 +2750,19 @@
         <v>162</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>163</v>
       </c>
       <c r="E32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>164</v>
@@ -2779,19 +2779,19 @@
         <v>165</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>165</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>166</v>
@@ -2808,19 +2808,19 @@
         <v>168</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>170</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>171</v>
@@ -2837,19 +2837,19 @@
         <v>173</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>175</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>176</v>
@@ -2866,19 +2866,19 @@
         <v>178</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>184</v>
@@ -2895,19 +2895,19 @@
         <v>468</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>187</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>189</v>
@@ -2924,19 +2924,19 @@
         <v>190</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>191</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>192</v>
@@ -2953,19 +2953,19 @@
         <v>194</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>194</v>
       </c>
       <c r="E39" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>196</v>
@@ -2982,19 +2982,19 @@
         <v>198</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>200</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>201</v>
@@ -3011,19 +3011,19 @@
         <v>202</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>204</v>
       </c>
       <c r="E41" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>205</v>
@@ -3040,19 +3040,19 @@
         <v>207</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>208</v>
       </c>
       <c r="E42" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>209</v>
@@ -3069,19 +3069,19 @@
         <v>210</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>212</v>
       </c>
       <c r="E43" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>214</v>
@@ -3098,19 +3098,19 @@
         <v>216</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>218</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>219</v>
       </c>
       <c r="E44" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F44" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>220</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>221</v>
@@ -3127,19 +3127,19 @@
         <v>222</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>224</v>
       </c>
       <c r="E45" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>225</v>
@@ -3156,19 +3156,19 @@
         <v>227</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>228</v>
       </c>
       <c r="E46" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>229</v>
@@ -3185,19 +3185,19 @@
         <v>231</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>233</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>235</v>
@@ -3214,19 +3214,19 @@
         <v>237</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>239</v>
       </c>
       <c r="E48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>241</v>
@@ -3243,19 +3243,19 @@
         <v>243</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>245</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>246</v>
       </c>
       <c r="E49" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F49" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>248</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>249</v>
@@ -3272,19 +3272,19 @@
         <v>250</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E50" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>252</v>
@@ -3301,19 +3301,19 @@
         <v>253</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>254</v>
       </c>
       <c r="E51" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>255</v>
@@ -3330,19 +3330,19 @@
         <v>256</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>257</v>
       </c>
       <c r="E52" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>258</v>
@@ -3359,19 +3359,19 @@
         <v>260</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>260</v>
       </c>
       <c r="E53" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>261</v>
@@ -3388,19 +3388,19 @@
         <v>263</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>264</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>265</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>266</v>
       </c>
       <c r="E54" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>264</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>267</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>268</v>
@@ -3417,19 +3417,19 @@
         <v>269</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>270</v>
       </c>
       <c r="E55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>271</v>
@@ -3446,19 +3446,19 @@
         <v>273</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>274</v>
       </c>
       <c r="E56" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>275</v>
@@ -3475,19 +3475,19 @@
         <v>276</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>277</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>278</v>
       </c>
       <c r="E57" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" s="4" t="s">
         <v>279</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>280</v>
@@ -3504,19 +3504,19 @@
         <v>281</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>283</v>
       </c>
       <c r="E58" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F58" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>284</v>
@@ -3533,19 +3533,19 @@
         <v>285</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>287</v>
       </c>
       <c r="E59" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>288</v>
@@ -3562,19 +3562,19 @@
         <v>289</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>290</v>
       </c>
       <c r="E60" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>291</v>
@@ -3591,19 +3591,19 @@
         <v>292</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>292</v>
       </c>
       <c r="E61" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F61" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>293</v>
@@ -3620,19 +3620,19 @@
         <v>294</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>295</v>
       </c>
       <c r="E62" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>296</v>
@@ -3649,19 +3649,19 @@
         <v>298</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>300</v>
       </c>
       <c r="E63" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F63" s="4" t="s">
         <v>301</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>302</v>
@@ -3678,19 +3678,19 @@
         <v>303</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>305</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>306</v>
       </c>
       <c r="E64" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F64" s="4" t="s">
         <v>307</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>308</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>309</v>
@@ -3707,19 +3707,19 @@
         <v>311</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>313</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>314</v>
       </c>
       <c r="E65" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F65" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>315</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>316</v>
@@ -3736,19 +3736,19 @@
         <v>317</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>318</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>319</v>
       </c>
       <c r="E66" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F66" s="4" t="s">
         <v>318</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>320</v>
@@ -3765,19 +3765,19 @@
         <v>321</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>322</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>323</v>
       </c>
       <c r="E67" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F67" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>325</v>
@@ -3794,19 +3794,19 @@
         <v>326</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>327</v>
       </c>
       <c r="E68" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F68" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>328</v>
@@ -3823,19 +3823,19 @@
         <v>330</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>331</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>332</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>333</v>
       </c>
       <c r="E69" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F69" s="4" t="s">
         <v>331</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>335</v>
@@ -3852,19 +3852,19 @@
         <v>336</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>332</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>336</v>
       </c>
       <c r="E70" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F70" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>337</v>
@@ -3881,19 +3881,19 @@
         <v>339</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>332</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>339</v>
       </c>
       <c r="E71" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F71" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>340</v>
@@ -3910,19 +3910,19 @@
         <v>342</v>
       </c>
       <c r="B72" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>343</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>344</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>342</v>
       </c>
       <c r="E72" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="F72" s="4" t="s">
         <v>343</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>345</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>346</v>
@@ -3939,19 +3939,19 @@
         <v>347</v>
       </c>
       <c r="B73" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>348</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>349</v>
       </c>
       <c r="E73" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F73" s="4" t="s">
         <v>348</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>350</v>
@@ -3968,19 +3968,19 @@
         <v>352</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>354</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>355</v>
       </c>
       <c r="E74" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F74" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>356</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>357</v>
@@ -3997,19 +3997,19 @@
         <v>358</v>
       </c>
       <c r="B75" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>359</v>
       </c>
       <c r="E75" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F75" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>360</v>
@@ -4026,19 +4026,19 @@
         <v>361</v>
       </c>
       <c r="B76" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>362</v>
       </c>
       <c r="E76" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F76" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>363</v>
@@ -4055,19 +4055,19 @@
         <v>365</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>366</v>
       </c>
       <c r="E77" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>367</v>
@@ -4084,19 +4084,19 @@
         <v>369</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>370</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>332</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>371</v>
       </c>
       <c r="E78" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F78" s="4" t="s">
         <v>370</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>372</v>
@@ -4113,19 +4113,19 @@
         <v>374</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>375</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>376</v>
       </c>
       <c r="E79" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F79" s="4" t="s">
         <v>377</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>378</v>
@@ -4142,19 +4142,19 @@
         <v>380</v>
       </c>
       <c r="B80" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>381</v>
       </c>
       <c r="E80" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F80" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>382</v>
@@ -4171,19 +4171,19 @@
         <v>383</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>384</v>
       </c>
       <c r="E81" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F81" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="F81" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>385</v>
@@ -4200,19 +4200,19 @@
         <v>387</v>
       </c>
       <c r="B82" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>388</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>389</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>390</v>
       </c>
       <c r="E82" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F82" s="4" t="s">
         <v>391</v>
-      </c>
-      <c r="F82" s="4" t="s">
-        <v>392</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>393</v>
@@ -4229,19 +4229,19 @@
         <v>395</v>
       </c>
       <c r="B83" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>322</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>396</v>
       </c>
       <c r="E83" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F83" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>397</v>
@@ -4258,19 +4258,19 @@
         <v>399</v>
       </c>
       <c r="B84" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>400</v>
       </c>
       <c r="E84" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>401</v>
@@ -4287,19 +4287,19 @@
         <v>403</v>
       </c>
       <c r="B85" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C85" s="4" t="s">
         <v>404</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>405</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>406</v>
       </c>
       <c r="E85" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F85" s="4" t="s">
         <v>404</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>405</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>407</v>
@@ -4316,19 +4316,19 @@
         <v>408</v>
       </c>
       <c r="B86" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>409</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>410</v>
       </c>
       <c r="D86" s="10" t="s">
         <v>408</v>
       </c>
       <c r="E86" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>409</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>411</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>412</v>
@@ -4345,19 +4345,19 @@
         <v>413</v>
       </c>
       <c r="B87" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>413</v>
       </c>
       <c r="E87" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F87" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>414</v>
@@ -4372,19 +4372,19 @@
         <v>415</v>
       </c>
       <c r="B88" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>416</v>
       </c>
       <c r="E88" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F88" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>417</v>
@@ -4399,19 +4399,19 @@
         <v>418</v>
       </c>
       <c r="B89" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>418</v>
       </c>
       <c r="E89" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F89" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>419</v>
@@ -4428,19 +4428,19 @@
         <v>420</v>
       </c>
       <c r="B90" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>421</v>
       </c>
       <c r="E90" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F90" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F90" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>422</v>
@@ -4457,19 +4457,19 @@
         <v>424</v>
       </c>
       <c r="B91" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>425</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>305</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>426</v>
       </c>
       <c r="E91" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F91" s="4" t="s">
         <v>427</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>308</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>428</v>
@@ -4486,19 +4486,19 @@
         <v>430</v>
       </c>
       <c r="B92" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>431</v>
       </c>
       <c r="E92" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F92" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>432</v>
@@ -4515,19 +4515,19 @@
         <v>433</v>
       </c>
       <c r="B93" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>435</v>
       </c>
       <c r="E93" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F93" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>436</v>
@@ -4544,19 +4544,19 @@
         <v>438</v>
       </c>
       <c r="B94" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>438</v>
       </c>
       <c r="E94" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F94" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="F94" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>439</v>
@@ -4573,19 +4573,19 @@
         <v>440</v>
       </c>
       <c r="B95" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>441</v>
       </c>
       <c r="E95" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>442</v>
@@ -4602,19 +4602,19 @@
         <v>444</v>
       </c>
       <c r="B96" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C96" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>445</v>
       </c>
       <c r="E96" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F96" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="F96" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>446</v>
@@ -4631,19 +4631,19 @@
         <v>447</v>
       </c>
       <c r="B97" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C97" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>245</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>448</v>
       </c>
       <c r="E97" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F97" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="F97" s="4" t="s">
-        <v>248</v>
       </c>
       <c r="G97" s="5" t="s">
         <v>449</v>
@@ -4660,19 +4660,19 @@
         <v>450</v>
       </c>
       <c r="B98" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="C98" s="4" t="s">
         <v>451</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>452</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>450</v>
       </c>
       <c r="E98" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="F98" s="4" t="s">
         <v>451</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>453</v>
       </c>
       <c r="G98" s="5" t="s">
         <v>454</v>
@@ -4689,19 +4689,19 @@
         <v>455</v>
       </c>
       <c r="B99" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C99" s="4" t="s">
         <v>456</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>245</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>457</v>
       </c>
       <c r="E99" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F99" s="4" t="s">
         <v>458</v>
-      </c>
-      <c r="F99" s="4" t="s">
-        <v>248</v>
       </c>
       <c r="G99" s="5" t="s">
         <v>459</v>
@@ -4718,19 +4718,19 @@
         <v>460</v>
       </c>
       <c r="B100" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C100" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>461</v>
       </c>
       <c r="E100" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F100" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F100" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G100" s="5" t="s">
         <v>462</v>
@@ -4747,19 +4747,19 @@
         <v>464</v>
       </c>
       <c r="B101" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C101" s="4" t="s">
         <v>465</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>466</v>
       </c>
       <c r="E101" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F101" s="4" t="s">
         <v>465</v>
-      </c>
-      <c r="F101" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="G101" s="5" t="s">
         <v>467</v>
@@ -4777,6 +4777,6 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="66" fitToHeight="2" orientation="portrait" horizontalDpi="4294967294"/>
+  <pageSetup paperSize="9" scale="66" fitToHeight="2" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>